<commit_message>
add new entry in gitignore, modification in analysis.
</commit_message>
<xml_diff>
--- a/outputs/02_datasets_statistics/analysis1.xlsx
+++ b/outputs/02_datasets_statistics/analysis1.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PedroPauloFavatoBarc\Dev\er2025data\outputs\02_datasets_statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DE9313-9CCD-4200-A4C5-D8E85B8A8342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D4541C-28C7-49DA-9ABB-86700EA2D9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{27C5B39C-A0F1-43C0-8CDE-04F4A5A81756}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{27C5B39C-A0F1-43C0-8CDE-04F4A5A81756}"/>
   </bookViews>
   <sheets>
-    <sheet name="c_rank_mc" sheetId="4" r:id="rId1"/>
-    <sheet name="c_rank_af" sheetId="3" r:id="rId2"/>
+    <sheet name="c_rank_af" sheetId="3" r:id="rId1"/>
+    <sheet name="c_rank_mc" sheetId="4" r:id="rId2"/>
     <sheet name="r_rank_af" sheetId="1" r:id="rId3"/>
     <sheet name="r_rank_mc" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="59">
   <si>
     <t>Stereotype</t>
   </si>
@@ -192,13 +193,37 @@
   </si>
   <si>
     <t>subkind</t>
+  </si>
+  <si>
+    <t>Class AF median</t>
+  </si>
+  <si>
+    <t>Class MC median</t>
+  </si>
+  <si>
+    <t>Above Median</t>
+  </si>
+  <si>
+    <t>Relation AF median</t>
+  </si>
+  <si>
+    <t>Relation MC median</t>
+  </si>
+  <si>
+    <t>Top Used</t>
+  </si>
+  <si>
+    <t>Core Relation</t>
+  </si>
+  <si>
+    <t>Core Class</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +232,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -235,19 +268,337 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="43">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -261,15 +612,6 @@
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="-1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -288,50 +630,68 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3EBD4CB8-38DE-443E-A7DE-0FDA907E5371}" name="Table15" displayName="Table15" ref="A1:F22" totalsRowShown="0">
-  <autoFilter ref="A1:F22" xr:uid="{2FD1A0A0-0AF6-49F2-8941-530D1F37F151}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53AA1836-20AF-491D-A134-5753818AC132}" name="Table24" displayName="Table24" ref="A1:H22" totalsRowShown="0">
+  <autoFilter ref="A1:H22" xr:uid="{65263D4F-6C0E-493E-83B6-7A1994F2218B}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{F1954C0B-54C4-418E-8B3F-FBA9B1F53354}" name="Stereotype"/>
+    <tableColumn id="2" xr3:uid="{C1917E6F-D0E7-4632-B782-68BDF9F2DABF}" name="Frequency"/>
+    <tableColumn id="3" xr3:uid="{776BB365-C128-49F1-A318-BFBEA147C83D}" name="Rank"/>
+    <tableColumn id="4" xr3:uid="{8FC3216D-E27A-4EA5-9026-919C76A75979}" name="Cumulative Frequency"/>
+    <tableColumn id="5" xr3:uid="{11FFA945-12D9-42C8-BB51-25D63BAE5D55}" name="Cumulative Percentage" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{14150508-81C1-433A-BF2E-348653799B3A}" name="Individual" dataDxfId="40">
+      <calculatedColumnFormula>Table24[[#This Row],[Cumulative Percentage]]-E1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{C605A4C1-C2DF-4485-AE1F-73803EB75CBF}" name="Above Median" dataDxfId="34">
+      <calculatedColumnFormula>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{F9B2D2F8-0ECE-461B-BB38-29D122623727}" name="Top Used" dataDxfId="30">
+      <calculatedColumnFormula>IF(SUM($F$2:$F2)&lt;=$K$2,TRUE,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3EBD4CB8-38DE-443E-A7DE-0FDA907E5371}" name="Table15" displayName="Table15" ref="A1:H22" totalsRowShown="0">
+  <autoFilter ref="A1:H22" xr:uid="{2FD1A0A0-0AF6-49F2-8941-530D1F37F151}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{EE094366-FE02-478D-9EB9-2B5816FC7CBA}" name="Stereotype"/>
     <tableColumn id="2" xr3:uid="{DB54A924-7FCF-4B82-BB96-71ECD2C6E785}" name="Group-wise Frequency"/>
     <tableColumn id="3" xr3:uid="{A0A0A04C-6C42-494F-A94D-B817FEB931B1}" name="Group-wise Rank"/>
     <tableColumn id="4" xr3:uid="{9C32FBA7-38F0-4AB9-A79C-970F90124943}" name="Cumulative Group-wise Frequency"/>
-    <tableColumn id="5" xr3:uid="{84588263-E122-4048-817D-CB2F1D166C9E}" name="Group-wise Cumulative Percentage" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{A5B9E1CD-8765-434F-8225-93129AA02A13}" name="Individual" dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{84588263-E122-4048-817D-CB2F1D166C9E}" name="Group-wise Cumulative Percentage" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{A5B9E1CD-8765-434F-8225-93129AA02A13}" name="Individual" dataDxfId="25">
       <calculatedColumnFormula>Table15[[#This Row],[Group-wise Cumulative Percentage]]-E1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{A929140B-8E95-439C-9E44-FC9B88523A08}" name="Above Median" dataDxfId="35">
+      <calculatedColumnFormula>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{1AE06D33-F208-4380-A312-C9F1543306A8}" name="Top Used">
+      <calculatedColumnFormula>IF(SUM($F$2:$F2)&lt;=$K$2,TRUE,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53AA1836-20AF-491D-A134-5753818AC132}" name="Table24" displayName="Table24" ref="A1:F22" totalsRowShown="0">
-  <autoFilter ref="A1:F22" xr:uid="{65263D4F-6C0E-493E-83B6-7A1994F2218B}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F1954C0B-54C4-418E-8B3F-FBA9B1F53354}" name="Stereotype"/>
-    <tableColumn id="2" xr3:uid="{C1917E6F-D0E7-4632-B782-68BDF9F2DABF}" name="Frequency"/>
-    <tableColumn id="3" xr3:uid="{776BB365-C128-49F1-A318-BFBEA147C83D}" name="Rank"/>
-    <tableColumn id="4" xr3:uid="{8FC3216D-E27A-4EA5-9026-919C76A75979}" name="Cumulative Frequency"/>
-    <tableColumn id="5" xr3:uid="{11FFA945-12D9-42C8-BB51-25D63BAE5D55}" name="Cumulative Percentage" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{14150508-81C1-433A-BF2E-348653799B3A}" name="Individual" dataDxfId="2">
-      <calculatedColumnFormula>Table24[[#This Row],[Cumulative Percentage]]-E1</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{07A21779-B4B2-4AA5-984F-5C55254B76CF}" name="Table1" displayName="Table1" ref="A1:F21" totalsRowShown="0">
-  <autoFilter ref="A1:F21" xr:uid="{07A21779-B4B2-4AA5-984F-5C55254B76CF}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{07A21779-B4B2-4AA5-984F-5C55254B76CF}" name="Table1" displayName="Table1" ref="A1:H21" totalsRowShown="0">
+  <autoFilter ref="A1:H21" xr:uid="{07A21779-B4B2-4AA5-984F-5C55254B76CF}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{E6CBD642-118E-41F5-8D02-A98174AFD92E}" name="Stereotype"/>
     <tableColumn id="2" xr3:uid="{F4FB94A8-EA74-4561-A6EF-50F6CC1D9414}" name="Frequency"/>
     <tableColumn id="3" xr3:uid="{A8925ECC-FBAE-419A-A525-5ADF915D7C72}" name="Rank"/>
     <tableColumn id="4" xr3:uid="{596C3938-7E79-42E7-B614-22587BAC3DCD}" name="Cumulative Frequency"/>
-    <tableColumn id="5" xr3:uid="{47E4A132-8A2E-47C9-B213-5904B26CD7B4}" name="Cumulative Percentage" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{5CB72DBB-92B8-4F51-8CF0-A6D8BF383B07}" name="Individual" dataDxfId="6">
+    <tableColumn id="5" xr3:uid="{47E4A132-8A2E-47C9-B213-5904B26CD7B4}" name="Cumulative Percentage" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{5CB72DBB-92B8-4F51-8CF0-A6D8BF383B07}" name="Individual" dataDxfId="38">
       <calculatedColumnFormula>Table1[[#This Row],[Cumulative Percentage]]-E1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{3F496BC5-E737-4545-B2ED-AC7D2E3C8FDA}" name="Above Median" dataDxfId="33">
+      <calculatedColumnFormula>IF(Table1[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{E01FDC1E-70F0-413E-8EB8-6E6CD7E74BFB}" name="Top Used" dataDxfId="31">
+      <calculatedColumnFormula>IF(SUM($F$2:$F2)&lt;=$K$2,TRUE,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -339,16 +699,22 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AA0108CD-0580-4A38-85A1-591D9E464710}" name="Table2" displayName="Table2" ref="A1:F21" totalsRowShown="0">
-  <autoFilter ref="A1:F21" xr:uid="{AA0108CD-0580-4A38-85A1-591D9E464710}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AA0108CD-0580-4A38-85A1-591D9E464710}" name="Table2" displayName="Table2" ref="A1:H21" totalsRowShown="0">
+  <autoFilter ref="A1:H21" xr:uid="{AA0108CD-0580-4A38-85A1-591D9E464710}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{B3F62159-E19D-4833-8558-8F6A42D1369C}" name="Stereotype"/>
     <tableColumn id="2" xr3:uid="{2FE17696-5E2F-44CE-A728-70C14892B94B}" name="Group-wise Frequency"/>
     <tableColumn id="3" xr3:uid="{D280B8A1-E902-48ED-83F1-5F50C03B5AC1}" name="Group-wise Rank"/>
     <tableColumn id="4" xr3:uid="{C29C325E-2C3D-48A0-9E9A-F89B4C87BCA3}" name="Cumulative Group-wise Frequency"/>
-    <tableColumn id="5" xr3:uid="{79828A7A-41CA-4674-875A-DB380C80803E}" name="Group-wise Cumulative Percentage" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{B30AB98A-FCCF-47FD-B00B-39BE50E9553E}" name="Individual" dataDxfId="4">
+    <tableColumn id="5" xr3:uid="{79828A7A-41CA-4674-875A-DB380C80803E}" name="Group-wise Cumulative Percentage" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{B30AB98A-FCCF-47FD-B00B-39BE50E9553E}" name="Individual" dataDxfId="36">
       <calculatedColumnFormula>Table2[[#This Row],[Group-wise Cumulative Percentage]]-E1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{9160CA11-241A-4ED5-8AC1-55F9F1017623}" name="Above Median" dataDxfId="32">
+      <calculatedColumnFormula>IF(Table2[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{7905A15A-6A6F-4A77-888E-902775D81F22}" name="Top Used">
+      <calculatedColumnFormula>IF(SUM($F$2:$F2)&lt;=$K$2,TRUE,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -671,11 +1037,708 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94DBF66-F2AD-4E29-AF11-71C77B0013D0}">
-  <dimension ref="A1:H22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB12ED2-62FA-45C7-8F3B-D5C22AE2FABF}">
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="A12" sqref="A2:A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="5" width="20.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="11" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1">
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2">
+        <v>2105</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2105</v>
+      </c>
+      <c r="E2" s="2">
+        <v>19.363444025388599</v>
+      </c>
+      <c r="F2" s="2">
+        <f>ROUND(Table24[[#This Row],[Cumulative Percentage]],2)</f>
+        <v>19.36</v>
+      </c>
+      <c r="G2" t="b">
+        <f>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <f>IF(SUM($F$2:$F2)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2">
+        <v>97.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3">
+        <v>1901</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>4006</v>
+      </c>
+      <c r="E3" s="2">
+        <v>36.850335755680199</v>
+      </c>
+      <c r="F3" s="2">
+        <f>ROUND(Table24[[#This Row],[Cumulative Percentage]]-E2,2)</f>
+        <v>17.489999999999998</v>
+      </c>
+      <c r="G3" t="b">
+        <f>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <f>IF(SUM($F$2:$F3)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4">
+        <v>1642</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>5648</v>
+      </c>
+      <c r="E4" s="2">
+        <v>51.954741974059402</v>
+      </c>
+      <c r="F4" s="2">
+        <f>ROUND(Table24[[#This Row],[Cumulative Percentage]]-E3,2)</f>
+        <v>15.1</v>
+      </c>
+      <c r="G4" t="b">
+        <f>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H4" t="b">
+        <f>IF(SUM($F$2:$F4)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5">
+        <v>1286</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>6934</v>
+      </c>
+      <c r="E5" s="2">
+        <v>63.784380461779001</v>
+      </c>
+      <c r="F5" s="2">
+        <f>ROUND(Table24[[#This Row],[Cumulative Percentage]]-E4,2)</f>
+        <v>11.83</v>
+      </c>
+      <c r="G5" t="b">
+        <f>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H5" t="b">
+        <f>IF(SUM($F$2:$F5)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6">
+        <v>622</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>7556</v>
+      </c>
+      <c r="E6" s="2">
+        <v>69.506025204672895</v>
+      </c>
+      <c r="F6" s="2">
+        <f>ROUND(Table24[[#This Row],[Cumulative Percentage]]-E5,2)</f>
+        <v>5.72</v>
+      </c>
+      <c r="G6" t="b">
+        <f>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <f>IF(SUM($F$2:$F6)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7">
+        <v>614</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>8170</v>
+      </c>
+      <c r="E7" s="2">
+        <v>75.154079661484602</v>
+      </c>
+      <c r="F7" s="2">
+        <f>ROUND(Table24[[#This Row],[Cumulative Percentage]]-E6,2)</f>
+        <v>5.65</v>
+      </c>
+      <c r="G7" t="b">
+        <f>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H7" t="b">
+        <f>IF(SUM($F$2:$F7)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8">
+        <v>598</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>8768</v>
+      </c>
+      <c r="E8" s="2">
+        <v>80.654953546131907</v>
+      </c>
+      <c r="F8" s="2">
+        <f>ROUND(Table24[[#This Row],[Cumulative Percentage]]-E7,2)</f>
+        <v>5.5</v>
+      </c>
+      <c r="G8" t="b">
+        <f>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H8" t="b">
+        <f>IF(SUM($F$2:$F8)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9">
+        <v>580</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>9348</v>
+      </c>
+      <c r="E9" s="2">
+        <v>85.990249287094102</v>
+      </c>
+      <c r="F9" s="2">
+        <f>ROUND(Table24[[#This Row],[Cumulative Percentage]]-E8,2)</f>
+        <v>5.34</v>
+      </c>
+      <c r="G9" t="b">
+        <f>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H9" t="b">
+        <f>IF(SUM($F$2:$F9)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10">
+        <v>361</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>9709</v>
+      </c>
+      <c r="E10" s="2">
+        <v>89.311010946555001</v>
+      </c>
+      <c r="F10" s="2">
+        <f>ROUND(Table24[[#This Row],[Cumulative Percentage]]-E9,2)</f>
+        <v>3.32</v>
+      </c>
+      <c r="G10" t="b">
+        <f>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H10" t="b">
+        <f>IF(SUM($F$2:$F10)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11">
+        <v>270</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>9979</v>
+      </c>
+      <c r="E11" s="2">
+        <v>91.794683101830501</v>
+      </c>
+      <c r="F11" s="2">
+        <f>ROUND(Table24[[#This Row],[Cumulative Percentage]]-E10,2)</f>
+        <v>2.48</v>
+      </c>
+      <c r="G11" t="b">
+        <f>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H11" t="b">
+        <f>IF(SUM($F$2:$F11)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12">
+        <v>266</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>10245</v>
+      </c>
+      <c r="E12" s="2">
+        <v>94.241560114064896</v>
+      </c>
+      <c r="F12" s="2">
+        <f>ROUND(Table24[[#This Row],[Cumulative Percentage]]-E11,2)</f>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="G12" t="b">
+        <f>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H12" t="b">
+        <f>IF(SUM($F$2:$F12)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13">
+        <v>134</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>10379</v>
+      </c>
+      <c r="E13" s="2">
+        <v>95.474197405942405</v>
+      </c>
+      <c r="F13" s="2">
+        <f>ROUND(Table24[[#This Row],[Cumulative Percentage]]-E12,2)</f>
+        <v>1.23</v>
+      </c>
+      <c r="G13" t="b">
+        <f>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" t="b">
+        <f>IF(SUM($F$2:$F13)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14">
+        <v>103</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>10482</v>
+      </c>
+      <c r="E14" s="2">
+        <v>96.421672339251202</v>
+      </c>
+      <c r="F14" s="2">
+        <f>ROUND(Table24[[#This Row],[Cumulative Percentage]]-E13,2)</f>
+        <v>0.95</v>
+      </c>
+      <c r="G14" t="b">
+        <f>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <f>IF(SUM($F$2:$F14)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15">
+        <v>90</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <v>10572</v>
+      </c>
+      <c r="E15" s="2">
+        <v>97.249563057676397</v>
+      </c>
+      <c r="F15" s="2">
+        <f>ROUND(Table24[[#This Row],[Cumulative Percentage]]-E14,2)</f>
+        <v>0.83</v>
+      </c>
+      <c r="G15" t="b">
+        <f>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" t="b">
+        <f>IF(SUM($F$2:$F15)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16">
+        <v>87</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <v>10659</v>
+      </c>
+      <c r="E16" s="2">
+        <v>98.049857418820693</v>
+      </c>
+      <c r="F16" s="2">
+        <f>ROUND(Table24[[#This Row],[Cumulative Percentage]]-E15,2)</f>
+        <v>0.8</v>
+      </c>
+      <c r="G16" t="b">
+        <f>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" t="b">
+        <f>IF(SUM($F$2:$F16)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17">
+        <v>75</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>10734</v>
+      </c>
+      <c r="E17" s="2">
+        <v>98.739766350841606</v>
+      </c>
+      <c r="F17" s="2">
+        <f>ROUND(Table24[[#This Row],[Cumulative Percentage]]-E16,2)</f>
+        <v>0.69</v>
+      </c>
+      <c r="G17" t="b">
+        <f>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H17" t="b">
+        <f>IF(SUM($F$2:$F17)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18">
+        <v>51</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <v>10785</v>
+      </c>
+      <c r="E18" s="2">
+        <v>99.208904424615895</v>
+      </c>
+      <c r="F18" s="2">
+        <f>ROUND(Table24[[#This Row],[Cumulative Percentage]]-E17,2)</f>
+        <v>0.47</v>
+      </c>
+      <c r="G18" t="b">
+        <f>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" t="b">
+        <f>IF(SUM($F$2:$F18)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19">
+        <v>46</v>
+      </c>
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <v>10831</v>
+      </c>
+      <c r="E19" s="2">
+        <v>99.632048569588804</v>
+      </c>
+      <c r="F19" s="2">
+        <f>ROUND(Table24[[#This Row],[Cumulative Percentage]]-E18,2)</f>
+        <v>0.42</v>
+      </c>
+      <c r="G19" t="b">
+        <f>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
+        <f>IF(SUM($F$2:$F19)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <v>10851</v>
+      </c>
+      <c r="E20" s="2">
+        <v>99.816024284794395</v>
+      </c>
+      <c r="F20" s="2">
+        <f>ROUND(Table24[[#This Row],[Cumulative Percentage]]-E19,2)</f>
+        <v>0.18</v>
+      </c>
+      <c r="G20" t="b">
+        <f>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H20" t="b">
+        <f>IF(SUM($F$2:$F20)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>10869</v>
+      </c>
+      <c r="E21" s="2">
+        <v>99.981602428479405</v>
+      </c>
+      <c r="F21" s="2">
+        <f>ROUND(Table24[[#This Row],[Cumulative Percentage]]-E20,2)</f>
+        <v>0.17</v>
+      </c>
+      <c r="G21" t="b">
+        <f>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" t="b">
+        <f>IF(SUM($F$2:$F21)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>21</v>
+      </c>
+      <c r="D22">
+        <v>10871</v>
+      </c>
+      <c r="E22" s="2">
+        <v>100</v>
+      </c>
+      <c r="F22" s="2">
+        <f>ROUND(Table24[[#This Row],[Cumulative Percentage]]-E21,2)</f>
+        <v>0.02</v>
+      </c>
+      <c r="G22" t="b">
+        <f>IF(Table24[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H22" t="b">
+        <f>IF(SUM($F$2:$F22)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G2:G21 G22:H22">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H21">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J18:K28">
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F2:F22" calculatedColumn="1"/>
+  </ignoredErrors>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94DBF66-F2AD-4E29-AF11-71C77B0013D0}">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +1746,7 @@
     <col min="2" max="5" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -702,9 +1765,21 @@
       <c r="F1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1">
+        <v>3.66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B2">
@@ -720,12 +1795,26 @@
         <v>11.3821138211382</v>
       </c>
       <c r="F2" s="1">
-        <f>Table15[[#This Row],[Group-wise Cumulative Percentage]]</f>
-        <v>11.3821138211382</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+        <f>ROUND(Table15[[#This Row],[Group-wise Cumulative Percentage]],2)</f>
+        <v>11.38</v>
+      </c>
+      <c r="G2" t="b">
+        <f>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <f>IF(SUM($F$2:$F2)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2">
+        <v>92.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B3">
@@ -741,12 +1830,20 @@
         <v>21.747967479674699</v>
       </c>
       <c r="F3" s="1">
-        <f>Table15[[#This Row],[Group-wise Cumulative Percentage]]-E2</f>
-        <v>10.3658536585365</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+        <f>ROUND(Table15[[#This Row],[Group-wise Cumulative Percentage]]-E2,2)</f>
+        <v>10.37</v>
+      </c>
+      <c r="G3" t="b">
+        <f>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <f>IF(SUM($F$2:$F3)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B4">
@@ -762,12 +1859,20 @@
         <v>31.808943089430802</v>
       </c>
       <c r="F4" s="1">
-        <f>Table15[[#This Row],[Group-wise Cumulative Percentage]]-E3</f>
-        <v>10.060975609756103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+        <f>ROUND(Table15[[#This Row],[Group-wise Cumulative Percentage]]-E3,2)</f>
+        <v>10.06</v>
+      </c>
+      <c r="G4" t="b">
+        <f>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H4" t="b">
+        <f>IF(SUM($F$2:$F4)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B5">
@@ -783,12 +1888,20 @@
         <v>41.565040650406502</v>
       </c>
       <c r="F5" s="1">
-        <f>Table15[[#This Row],[Group-wise Cumulative Percentage]]-E4</f>
-        <v>9.7560975609757001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+        <f>ROUND(Table15[[#This Row],[Group-wise Cumulative Percentage]]-E4,2)</f>
+        <v>9.76</v>
+      </c>
+      <c r="G5" t="b">
+        <f>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H5" t="b">
+        <f>IF(SUM($F$2:$F5)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B6">
@@ -804,13 +1917,21 @@
         <v>51.016260162601597</v>
       </c>
       <c r="F6" s="1">
-        <f>Table15[[#This Row],[Group-wise Cumulative Percentage]]-E5</f>
-        <v>9.4512195121950953</v>
-      </c>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+        <f>ROUND(Table15[[#This Row],[Group-wise Cumulative Percentage]]-E5,2)</f>
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="G6" t="b">
+        <f>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <f>IF(SUM($F$2:$F6)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B7">
@@ -826,12 +1947,20 @@
         <v>57.723577235772296</v>
       </c>
       <c r="F7" s="1">
-        <f>Table15[[#This Row],[Group-wise Cumulative Percentage]]-E6</f>
-        <v>6.7073170731706995</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+        <f>ROUND(Table15[[#This Row],[Group-wise Cumulative Percentage]]-E6,2)</f>
+        <v>6.71</v>
+      </c>
+      <c r="G7" t="b">
+        <f>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H7" t="b">
+        <f>IF(SUM($F$2:$F7)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B8">
@@ -847,12 +1976,20 @@
         <v>64.126016260162601</v>
       </c>
       <c r="F8" s="1">
-        <f>Table15[[#This Row],[Group-wise Cumulative Percentage]]-E7</f>
-        <v>6.4024390243903042</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+        <f>ROUND(Table15[[#This Row],[Group-wise Cumulative Percentage]]-E7,2)</f>
+        <v>6.4</v>
+      </c>
+      <c r="G8" t="b">
+        <f>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H8" t="b">
+        <f>IF(SUM($F$2:$F8)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B9">
@@ -868,12 +2005,20 @@
         <v>70.426829268292593</v>
       </c>
       <c r="F9" s="1">
-        <f>Table15[[#This Row],[Group-wise Cumulative Percentage]]-E8</f>
-        <v>6.3008130081299925</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+        <f>ROUND(Table15[[#This Row],[Group-wise Cumulative Percentage]]-E8,2)</f>
+        <v>6.3</v>
+      </c>
+      <c r="G9" t="b">
+        <f>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H9" t="b">
+        <f>IF(SUM($F$2:$F9)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B10">
@@ -889,12 +2034,20 @@
         <v>75.609756097560904</v>
       </c>
       <c r="F10" s="1">
-        <f>Table15[[#This Row],[Group-wise Cumulative Percentage]]-E9</f>
-        <v>5.1829268292683111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+        <f>ROUND(Table15[[#This Row],[Group-wise Cumulative Percentage]]-E9,2)</f>
+        <v>5.18</v>
+      </c>
+      <c r="G10" t="b">
+        <f>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H10" t="b">
+        <f>IF(SUM($F$2:$F10)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B11">
@@ -910,12 +2063,20 @@
         <v>80.284552845528395</v>
       </c>
       <c r="F11" s="1">
-        <f>Table15[[#This Row],[Group-wise Cumulative Percentage]]-E10</f>
-        <v>4.6747967479674912</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+        <f>ROUND(Table15[[#This Row],[Group-wise Cumulative Percentage]]-E10,2)</f>
+        <v>4.67</v>
+      </c>
+      <c r="G11" t="b">
+        <f>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H11" t="b">
+        <f>IF(SUM($F$2:$F11)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B12">
@@ -931,11 +2092,19 @@
         <v>83.943089430894304</v>
       </c>
       <c r="F12" s="1">
-        <f>Table15[[#This Row],[Group-wise Cumulative Percentage]]-E11</f>
-        <v>3.6585365853659084</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <f>ROUND(Table15[[#This Row],[Group-wise Cumulative Percentage]]-E11,2)</f>
+        <v>3.66</v>
+      </c>
+      <c r="G12" t="b">
+        <f>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H12" t="b">
+        <f>IF(SUM($F$2:$F12)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -952,11 +2121,19 @@
         <v>87.398373983739802</v>
       </c>
       <c r="F13" s="1">
-        <f>Table15[[#This Row],[Group-wise Cumulative Percentage]]-E12</f>
-        <v>3.4552845528454981</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <f>ROUND(Table15[[#This Row],[Group-wise Cumulative Percentage]]-E12,2)</f>
+        <v>3.46</v>
+      </c>
+      <c r="G13" t="b">
+        <f>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" t="b">
+        <f>IF(SUM($F$2:$F13)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -973,11 +2150,19 @@
         <v>90.243902439024396</v>
       </c>
       <c r="F14" s="1">
-        <f>Table15[[#This Row],[Group-wise Cumulative Percentage]]-E13</f>
-        <v>2.8455284552845939</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <f>ROUND(Table15[[#This Row],[Group-wise Cumulative Percentage]]-E13,2)</f>
+        <v>2.85</v>
+      </c>
+      <c r="G14" t="b">
+        <f>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <f>IF(SUM($F$2:$F14)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -994,11 +2179,19 @@
         <v>92.682926829268297</v>
       </c>
       <c r="F15" s="1">
-        <f>Table15[[#This Row],[Group-wise Cumulative Percentage]]-E14</f>
-        <v>2.4390243902439011</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <f>ROUND(Table15[[#This Row],[Group-wise Cumulative Percentage]]-E14,2)</f>
+        <v>2.44</v>
+      </c>
+      <c r="G15" t="b">
+        <f>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" t="b">
+        <f>IF(SUM($F$2:$F15)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1015,11 +2208,19 @@
         <v>95.121951219512198</v>
       </c>
       <c r="F16" s="1">
-        <f>Table15[[#This Row],[Group-wise Cumulative Percentage]]-E15</f>
-        <v>2.4390243902439011</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <f>ROUND(Table15[[#This Row],[Group-wise Cumulative Percentage]]-E15,2)</f>
+        <v>2.44</v>
+      </c>
+      <c r="G16" t="b">
+        <f>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" t="b">
+        <f>IF(SUM($F$2:$F16)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1036,11 +2237,19 @@
         <v>96.443089430894304</v>
       </c>
       <c r="F17" s="1">
-        <f>Table15[[#This Row],[Group-wise Cumulative Percentage]]-E16</f>
-        <v>1.321138211382106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <f>ROUND(Table15[[#This Row],[Group-wise Cumulative Percentage]]-E16,2)</f>
+        <v>1.32</v>
+      </c>
+      <c r="G17" t="b">
+        <f>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H17" t="b">
+        <f>IF(SUM($F$2:$F17)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1057,11 +2266,19 @@
         <v>97.459349593495901</v>
       </c>
       <c r="F18" s="1">
-        <f>Table15[[#This Row],[Group-wise Cumulative Percentage]]-E17</f>
-        <v>1.016260162601597</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <f>ROUND(Table15[[#This Row],[Group-wise Cumulative Percentage]]-E17,2)</f>
+        <v>1.02</v>
+      </c>
+      <c r="G18" t="b">
+        <f>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" t="b">
+        <f>IF(SUM($F$2:$F18)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1078,11 +2295,19 @@
         <v>98.373983739837399</v>
       </c>
       <c r="F19" s="1">
-        <f>Table15[[#This Row],[Group-wise Cumulative Percentage]]-E18</f>
-        <v>0.91463414634149842</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <f>ROUND(Table15[[#This Row],[Group-wise Cumulative Percentage]]-E18,2)</f>
+        <v>0.91</v>
+      </c>
+      <c r="G19" t="b">
+        <f>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
+        <f>IF(SUM($F$2:$F19)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1099,11 +2324,19 @@
         <v>99.1869918699187</v>
       </c>
       <c r="F20" s="1">
-        <f>Table15[[#This Row],[Group-wise Cumulative Percentage]]-E19</f>
-        <v>0.81300813008130035</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <f>ROUND(Table15[[#This Row],[Group-wise Cumulative Percentage]]-E19,2)</f>
+        <v>0.81</v>
+      </c>
+      <c r="G20" t="b">
+        <f>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H20" t="b">
+        <f>IF(SUM($F$2:$F20)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1120,11 +2353,19 @@
         <v>99.796747967479604</v>
       </c>
       <c r="F21" s="1">
-        <f>Table15[[#This Row],[Group-wise Cumulative Percentage]]-E20</f>
-        <v>0.60975609756090421</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <f>ROUND(Table15[[#This Row],[Group-wise Cumulative Percentage]]-E20,2)</f>
+        <v>0.61</v>
+      </c>
+      <c r="G21" t="b">
+        <f>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" t="b">
+        <f>IF(SUM($F$2:$F21)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1141,502 +2382,48 @@
         <v>100</v>
       </c>
       <c r="F22" s="1">
-        <f>Table15[[#This Row],[Group-wise Cumulative Percentage]]-E21</f>
-        <v>0.20325203252039614</v>
+        <f>ROUND(Table15[[#This Row],[Group-wise Cumulative Percentage]]-E21,2)</f>
+        <v>0.2</v>
+      </c>
+      <c r="G22" t="b">
+        <f>IF(Table15[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H22" t="b">
+        <f>IF(SUM($F$2:$F22)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G2:G22">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H21">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB12ED2-62FA-45C7-8F3B-D5C22AE2FABF}">
-  <dimension ref="A1:J22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="5" width="20.85546875" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2">
-        <v>2105</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2105</v>
-      </c>
-      <c r="E2" s="2">
-        <v>19.363444025388599</v>
-      </c>
-      <c r="F2" s="2">
-        <f>Table24[[#This Row],[Cumulative Percentage]]</f>
-        <v>19.363444025388599</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3">
-        <v>1901</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>4006</v>
-      </c>
-      <c r="E3" s="2">
-        <v>36.850335755680199</v>
-      </c>
-      <c r="F3" s="2">
-        <f>Table24[[#This Row],[Cumulative Percentage]]-E2</f>
-        <v>17.4868917302916</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4">
-        <v>1642</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>5648</v>
-      </c>
-      <c r="E4" s="2">
-        <v>51.954741974059402</v>
-      </c>
-      <c r="F4" s="2">
-        <f>Table24[[#This Row],[Cumulative Percentage]]-E3</f>
-        <v>15.104406218379204</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5">
-        <v>1286</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>6934</v>
-      </c>
-      <c r="E5" s="2">
-        <v>63.784380461779001</v>
-      </c>
-      <c r="F5" s="2">
-        <f>Table24[[#This Row],[Cumulative Percentage]]-E4</f>
-        <v>11.829638487719599</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6">
-        <v>622</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>7556</v>
-      </c>
-      <c r="E6" s="2">
-        <v>69.506025204672895</v>
-      </c>
-      <c r="F6" s="2">
-        <f>Table24[[#This Row],[Cumulative Percentage]]-E5</f>
-        <v>5.7216447428938935</v>
-      </c>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7">
-        <v>614</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>8170</v>
-      </c>
-      <c r="E7" s="2">
-        <v>75.154079661484602</v>
-      </c>
-      <c r="F7" s="2">
-        <f>Table24[[#This Row],[Cumulative Percentage]]-E6</f>
-        <v>5.6480544568117068</v>
-      </c>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8">
-        <v>598</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-      <c r="D8">
-        <v>8768</v>
-      </c>
-      <c r="E8" s="2">
-        <v>80.654953546131907</v>
-      </c>
-      <c r="F8" s="2">
-        <f>Table24[[#This Row],[Cumulative Percentage]]-E7</f>
-        <v>5.5008738846473051</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9">
-        <v>580</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-      <c r="D9">
-        <v>9348</v>
-      </c>
-      <c r="E9" s="2">
-        <v>85.990249287094102</v>
-      </c>
-      <c r="F9" s="2">
-        <f>Table24[[#This Row],[Cumulative Percentage]]-E8</f>
-        <v>5.3352957409621951</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10">
-        <v>361</v>
-      </c>
-      <c r="C10">
-        <v>9</v>
-      </c>
-      <c r="D10">
-        <v>9709</v>
-      </c>
-      <c r="E10" s="2">
-        <v>89.311010946555001</v>
-      </c>
-      <c r="F10" s="2">
-        <f>Table24[[#This Row],[Cumulative Percentage]]-E9</f>
-        <v>3.3207616594608993</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11">
-        <v>270</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-      <c r="D11">
-        <v>9979</v>
-      </c>
-      <c r="E11" s="2">
-        <v>91.794683101830501</v>
-      </c>
-      <c r="F11" s="2">
-        <f>Table24[[#This Row],[Cumulative Percentage]]-E10</f>
-        <v>2.4836721552754994</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12">
-        <v>266</v>
-      </c>
-      <c r="C12">
-        <v>11</v>
-      </c>
-      <c r="D12">
-        <v>10245</v>
-      </c>
-      <c r="E12" s="2">
-        <v>94.241560114064896</v>
-      </c>
-      <c r="F12" s="2">
-        <f>Table24[[#This Row],[Cumulative Percentage]]-E11</f>
-        <v>2.4468770122343955</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13">
-        <v>134</v>
-      </c>
-      <c r="C13">
-        <v>12</v>
-      </c>
-      <c r="D13">
-        <v>10379</v>
-      </c>
-      <c r="E13" s="2">
-        <v>95.474197405942405</v>
-      </c>
-      <c r="F13" s="2">
-        <f>Table24[[#This Row],[Cumulative Percentage]]-E12</f>
-        <v>1.2326372918775093</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14">
-        <v>103</v>
-      </c>
-      <c r="C14">
-        <v>13</v>
-      </c>
-      <c r="D14">
-        <v>10482</v>
-      </c>
-      <c r="E14" s="2">
-        <v>96.421672339251202</v>
-      </c>
-      <c r="F14" s="2">
-        <f>Table24[[#This Row],[Cumulative Percentage]]-E13</f>
-        <v>0.94747493330879706</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15">
-        <v>90</v>
-      </c>
-      <c r="C15">
-        <v>14</v>
-      </c>
-      <c r="D15">
-        <v>10572</v>
-      </c>
-      <c r="E15" s="2">
-        <v>97.249563057676397</v>
-      </c>
-      <c r="F15" s="2">
-        <f>Table24[[#This Row],[Cumulative Percentage]]-E14</f>
-        <v>0.8278907184251949</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16">
-        <v>87</v>
-      </c>
-      <c r="C16">
-        <v>15</v>
-      </c>
-      <c r="D16">
-        <v>10659</v>
-      </c>
-      <c r="E16" s="2">
-        <v>98.049857418820693</v>
-      </c>
-      <c r="F16" s="2">
-        <f>Table24[[#This Row],[Cumulative Percentage]]-E15</f>
-        <v>0.80029436114429586</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17">
-        <v>75</v>
-      </c>
-      <c r="C17">
-        <v>16</v>
-      </c>
-      <c r="D17">
-        <v>10734</v>
-      </c>
-      <c r="E17" s="2">
-        <v>98.739766350841606</v>
-      </c>
-      <c r="F17" s="2">
-        <f>Table24[[#This Row],[Cumulative Percentage]]-E16</f>
-        <v>0.68990893202091286</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18">
-        <v>51</v>
-      </c>
-      <c r="C18">
-        <v>17</v>
-      </c>
-      <c r="D18">
-        <v>10785</v>
-      </c>
-      <c r="E18" s="2">
-        <v>99.208904424615895</v>
-      </c>
-      <c r="F18" s="2">
-        <f>Table24[[#This Row],[Cumulative Percentage]]-E17</f>
-        <v>0.46913807377428896</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19">
-        <v>46</v>
-      </c>
-      <c r="C19">
-        <v>18</v>
-      </c>
-      <c r="D19">
-        <v>10831</v>
-      </c>
-      <c r="E19" s="2">
-        <v>99.632048569588804</v>
-      </c>
-      <c r="F19" s="2">
-        <f>Table24[[#This Row],[Cumulative Percentage]]-E18</f>
-        <v>0.42314414497290898</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20">
-        <v>20</v>
-      </c>
-      <c r="C20">
-        <v>19</v>
-      </c>
-      <c r="D20">
-        <v>10851</v>
-      </c>
-      <c r="E20" s="2">
-        <v>99.816024284794395</v>
-      </c>
-      <c r="F20" s="2">
-        <f>Table24[[#This Row],[Cumulative Percentage]]-E19</f>
-        <v>0.18397571520559097</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21">
-        <v>18</v>
-      </c>
-      <c r="C21">
-        <v>20</v>
-      </c>
-      <c r="D21">
-        <v>10869</v>
-      </c>
-      <c r="E21" s="2">
-        <v>99.981602428479405</v>
-      </c>
-      <c r="F21" s="2">
-        <f>Table24[[#This Row],[Cumulative Percentage]]-E20</f>
-        <v>0.16557814368501056</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22">
-        <v>21</v>
-      </c>
-      <c r="D22">
-        <v>10871</v>
-      </c>
-      <c r="E22" s="2">
-        <v>100</v>
-      </c>
-      <c r="F22" s="2">
-        <f>Table24[[#This Row],[Cumulative Percentage]]-E21</f>
-        <v>1.8397571520594624E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F2:F22" calculatedColumn="1"/>
+  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -1645,20 +2432,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7657DF98-9C94-4A60-8FA0-AE51DE837BB4}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="5" width="20.85546875" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" customWidth="1"/>
+    <col min="6" max="11" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1677,9 +2464,21 @@
       <c r="F1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1">
+        <v>1.87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2">
@@ -1695,12 +2494,26 @@
         <v>35.8906525573192</v>
       </c>
       <c r="F2" s="1">
-        <f>Table1[[#This Row],[Cumulative Percentage]]</f>
-        <v>35.8906525573192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+        <f>ROUND(Table1[[#This Row],[Cumulative Percentage]],2)</f>
+        <v>35.89</v>
+      </c>
+      <c r="G2" t="b">
+        <f>IF(Table1[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <f>IF(SUM($F$2:$F2)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2">
+        <v>96.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B3">
@@ -1716,12 +2529,20 @@
         <v>47.742504409170998</v>
       </c>
       <c r="F3" s="1">
-        <f>Table1[[#This Row],[Cumulative Percentage]]-E2</f>
-        <v>11.851851851851798</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+        <f>ROUND(Table1[[#This Row],[Cumulative Percentage]]-E2,2)</f>
+        <v>11.85</v>
+      </c>
+      <c r="G3" t="b">
+        <f>IF(Table1[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <f>IF(SUM($F$2:$F3)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B4">
@@ -1737,12 +2558,20 @@
         <v>58.8888888888888</v>
       </c>
       <c r="F4" s="1">
-        <f>Table1[[#This Row],[Cumulative Percentage]]-E3</f>
-        <v>11.146384479717803</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+        <f>ROUND(Table1[[#This Row],[Cumulative Percentage]]-E3,2)</f>
+        <v>11.15</v>
+      </c>
+      <c r="G4" t="b">
+        <f>IF(Table1[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H4" t="b">
+        <f>IF(SUM($F$2:$F4)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B5">
@@ -1758,12 +2587,20 @@
         <v>68.800705467372097</v>
       </c>
       <c r="F5" s="1">
-        <f>Table1[[#This Row],[Cumulative Percentage]]-E4</f>
-        <v>9.9118165784832968</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+        <f>ROUND(Table1[[#This Row],[Cumulative Percentage]]-E4,2)</f>
+        <v>9.91</v>
+      </c>
+      <c r="G5" t="b">
+        <f>IF(Table1[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H5" t="b">
+        <f>IF(SUM($F$2:$F5)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B6">
@@ -1779,12 +2616,20 @@
         <v>75.714285714285694</v>
       </c>
       <c r="F6" s="1">
-        <f>Table1[[#This Row],[Cumulative Percentage]]-E5</f>
-        <v>6.9135802469135967</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+        <f>ROUND(Table1[[#This Row],[Cumulative Percentage]]-E5,2)</f>
+        <v>6.91</v>
+      </c>
+      <c r="G6" t="b">
+        <f>IF(Table1[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <f>IF(SUM($F$2:$F6)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B7">
@@ -1800,12 +2645,20 @@
         <v>80.564373897707199</v>
       </c>
       <c r="F7" s="1">
-        <f>Table1[[#This Row],[Cumulative Percentage]]-E6</f>
-        <v>4.8500881834215051</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+        <f>ROUND(Table1[[#This Row],[Cumulative Percentage]]-E6,2)</f>
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="G7" t="b">
+        <f>IF(Table1[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H7" t="b">
+        <f>IF(SUM($F$2:$F7)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B8">
@@ -1821,12 +2674,20 @@
         <v>84.4444444444444</v>
       </c>
       <c r="F8" s="1">
-        <f>Table1[[#This Row],[Cumulative Percentage]]-E7</f>
-        <v>3.8800705467372012</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+        <f>ROUND(Table1[[#This Row],[Cumulative Percentage]]-E7,2)</f>
+        <v>3.88</v>
+      </c>
+      <c r="G8" t="b">
+        <f>IF(Table1[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H8" t="b">
+        <f>IF(SUM($F$2:$F8)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B9">
@@ -1842,12 +2703,20 @@
         <v>88.042328042327995</v>
       </c>
       <c r="F9" s="1">
-        <f>Table1[[#This Row],[Cumulative Percentage]]-E8</f>
-        <v>3.5978835978835946</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+        <f>ROUND(Table1[[#This Row],[Cumulative Percentage]]-E8,2)</f>
+        <v>3.6</v>
+      </c>
+      <c r="G9" t="b">
+        <f>IF(Table1[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H9" t="b">
+        <f>IF(SUM($F$2:$F9)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B10">
@@ -1863,12 +2732,20 @@
         <v>90.317460317460302</v>
       </c>
       <c r="F10" s="1">
-        <f>Table1[[#This Row],[Cumulative Percentage]]-E9</f>
-        <v>2.2751322751323073</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+        <f>ROUND(Table1[[#This Row],[Cumulative Percentage]]-E9,2)</f>
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="G10" t="b">
+        <f>IF(Table1[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H10" t="b">
+        <f>IF(SUM($F$2:$F10)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B11">
@@ -1884,11 +2761,19 @@
         <v>92.310405643738903</v>
       </c>
       <c r="F11" s="1">
-        <f>Table1[[#This Row],[Cumulative Percentage]]-E10</f>
-        <v>1.9929453262786012</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <f>ROUND(Table1[[#This Row],[Cumulative Percentage]]-E10,2)</f>
+        <v>1.99</v>
+      </c>
+      <c r="G11" t="b">
+        <f>IF(Table1[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H11" t="b">
+        <f>IF(SUM($F$2:$F11)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1905,11 +2790,19 @@
         <v>94.056437389770693</v>
       </c>
       <c r="F12" s="1">
-        <f>Table1[[#This Row],[Cumulative Percentage]]-E11</f>
-        <v>1.7460317460317896</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <f>ROUND(Table1[[#This Row],[Cumulative Percentage]]-E11,2)</f>
+        <v>1.75</v>
+      </c>
+      <c r="G12" t="b">
+        <f>IF(Table1[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" t="b">
+        <f>IF(SUM($F$2:$F12)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1926,11 +2819,19 @@
         <v>95.308641975308603</v>
       </c>
       <c r="F13" s="1">
-        <f>Table1[[#This Row],[Cumulative Percentage]]-E12</f>
-        <v>1.2522045855379105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <f>ROUND(Table1[[#This Row],[Cumulative Percentage]]-E12,2)</f>
+        <v>1.25</v>
+      </c>
+      <c r="G13" t="b">
+        <f>IF(Table1[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" t="b">
+        <f>IF(SUM($F$2:$F13)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1947,11 +2848,19 @@
         <v>96.490299823633094</v>
       </c>
       <c r="F14" s="1">
-        <f>Table1[[#This Row],[Cumulative Percentage]]-E13</f>
-        <v>1.1816578483244911</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <f>ROUND(Table1[[#This Row],[Cumulative Percentage]]-E13,2)</f>
+        <v>1.18</v>
+      </c>
+      <c r="G14" t="b">
+        <f>IF(Table1[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <f>IF(SUM($F$2:$F14)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1968,11 +2877,19 @@
         <v>97.231040564373899</v>
       </c>
       <c r="F15" s="1">
-        <f>Table1[[#This Row],[Cumulative Percentage]]-E14</f>
-        <v>0.74074074074080443</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <f>ROUND(Table1[[#This Row],[Cumulative Percentage]]-E14,2)</f>
+        <v>0.74</v>
+      </c>
+      <c r="G15" t="b">
+        <f>IF(Table1[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" t="b">
+        <f>IF(SUM($F$2:$F15)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1989,11 +2906,19 @@
         <v>97.918871252204497</v>
       </c>
       <c r="F16" s="1">
-        <f>Table1[[#This Row],[Cumulative Percentage]]-E15</f>
-        <v>0.68783068783059775</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <f>ROUND(Table1[[#This Row],[Cumulative Percentage]]-E15,2)</f>
+        <v>0.69</v>
+      </c>
+      <c r="G16" t="b">
+        <f>IF(Table1[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" t="b">
+        <f>IF(SUM($F$2:$F16)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -2010,11 +2935,19 @@
         <v>98.589065255731896</v>
       </c>
       <c r="F17" s="1">
-        <f>Table1[[#This Row],[Cumulative Percentage]]-E16</f>
-        <v>0.67019400352739922</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <f>ROUND(Table1[[#This Row],[Cumulative Percentage]]-E16,2)</f>
+        <v>0.67</v>
+      </c>
+      <c r="G17" t="b">
+        <f>IF(Table1[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H17" t="b">
+        <f>IF(SUM($F$2:$F17)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -2031,11 +2964,19 @@
         <v>99.065255731922306</v>
       </c>
       <c r="F18" s="1">
-        <f>Table1[[#This Row],[Cumulative Percentage]]-E17</f>
-        <v>0.47619047619041055</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <f>ROUND(Table1[[#This Row],[Cumulative Percentage]]-E17,2)</f>
+        <v>0.48</v>
+      </c>
+      <c r="G18" t="b">
+        <f>IF(Table1[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" t="b">
+        <f>IF(SUM($F$2:$F18)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2052,11 +2993,19 @@
         <v>99.435626102292701</v>
       </c>
       <c r="F19" s="1">
-        <f>Table1[[#This Row],[Cumulative Percentage]]-E18</f>
-        <v>0.37037037037039511</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <f>ROUND(Table1[[#This Row],[Cumulative Percentage]]-E18,2)</f>
+        <v>0.37</v>
+      </c>
+      <c r="G19" t="b">
+        <f>IF(Table1[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
+        <f>IF(SUM($F$2:$F19)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2073,11 +3022,19 @@
         <v>99.753086419753004</v>
       </c>
       <c r="F20" s="1">
-        <f>Table1[[#This Row],[Cumulative Percentage]]-E19</f>
-        <v>0.31746031746030212</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <f>ROUND(Table1[[#This Row],[Cumulative Percentage]]-E19,2)</f>
+        <v>0.32</v>
+      </c>
+      <c r="G20" t="b">
+        <f>IF(Table1[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H20" t="b">
+        <f>IF(SUM($F$2:$F20)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -2094,13 +3051,32 @@
         <v>100</v>
       </c>
       <c r="F21" s="1">
-        <f>Table1[[#This Row],[Cumulative Percentage]]-E20</f>
-        <v>0.24691358024699639</v>
+        <f>ROUND(Table1[[#This Row],[Cumulative Percentage]]-E20,2)</f>
+        <v>0.25</v>
+      </c>
+      <c r="G21" t="b">
+        <f>IF(Table1[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" t="b">
+        <f>IF(SUM($F$2:$F21)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G2:H21">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F2:F21" calculatedColumn="1"/>
+  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -2109,18 +3085,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB6D174-19D8-4D59-8F79-51E260BAEA85}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="5" width="20.85546875" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" customWidth="1"/>
+    <col min="6" max="11" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2139,9 +3117,21 @@
       <c r="F1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1">
+        <v>4.12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2">
@@ -2157,12 +3147,26 @@
         <v>14.579759862778699</v>
       </c>
       <c r="F2" s="1">
-        <f>Table2[[#This Row],[Group-wise Cumulative Percentage]]</f>
-        <v>14.579759862778699</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+        <f>ROUND(Table2[[#This Row],[Group-wise Cumulative Percentage]],2)</f>
+        <v>14.58</v>
+      </c>
+      <c r="G2" t="b">
+        <f>IF(Table2[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <f>IF(SUM($F$2:$F2)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2">
+        <v>90.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B3">
@@ -2178,12 +3182,20 @@
         <v>28.130360205831899</v>
       </c>
       <c r="F3" s="1">
-        <f>Table2[[#This Row],[Group-wise Cumulative Percentage]]-E2</f>
-        <v>13.550600343053199</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+        <f>ROUND(Table2[[#This Row],[Group-wise Cumulative Percentage]]-E2,2)</f>
+        <v>13.55</v>
+      </c>
+      <c r="G3" t="b">
+        <f>IF(Table2[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <f>IF(SUM($F$2:$F3)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B4">
@@ -2199,12 +3211,20 @@
         <v>38.250428816466503</v>
       </c>
       <c r="F4" s="1">
-        <f>Table2[[#This Row],[Group-wise Cumulative Percentage]]-E3</f>
-        <v>10.120068610634604</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+        <f>ROUND(Table2[[#This Row],[Group-wise Cumulative Percentage]]-E3,2)</f>
+        <v>10.119999999999999</v>
+      </c>
+      <c r="G4" t="b">
+        <f>IF(Table2[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H4" t="b">
+        <f>IF(SUM($F$2:$F4)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B5">
@@ -2220,12 +3240,20 @@
         <v>46.483704974270999</v>
       </c>
       <c r="F5" s="1">
-        <f>Table2[[#This Row],[Group-wise Cumulative Percentage]]-E4</f>
-        <v>8.2332761578044966</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+        <f>ROUND(Table2[[#This Row],[Group-wise Cumulative Percentage]]-E4,2)</f>
+        <v>8.23</v>
+      </c>
+      <c r="G5" t="b">
+        <f>IF(Table2[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H5" t="b">
+        <f>IF(SUM($F$2:$F5)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B6">
@@ -2241,16 +3269,21 @@
         <v>53.344768439108002</v>
       </c>
       <c r="F6" s="1">
-        <f>Table2[[#This Row],[Group-wise Cumulative Percentage]]-E5</f>
-        <v>6.8610634648370024</v>
-      </c>
-      <c r="H6" s="3">
-        <f>(F2-Table2[[#This Row],[Individual]])/F2</f>
-        <v>0.52941176470588458</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+        <f>ROUND(Table2[[#This Row],[Group-wise Cumulative Percentage]]-E5,2)</f>
+        <v>6.86</v>
+      </c>
+      <c r="G6" t="b">
+        <f>IF(Table2[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <f>IF(SUM($F$2:$F6)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B7">
@@ -2266,12 +3299,20 @@
         <v>59.862778730703198</v>
       </c>
       <c r="F7" s="1">
-        <f>Table2[[#This Row],[Group-wise Cumulative Percentage]]-E6</f>
-        <v>6.5180102915951963</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+        <f>ROUND(Table2[[#This Row],[Group-wise Cumulative Percentage]]-E6,2)</f>
+        <v>6.52</v>
+      </c>
+      <c r="G7" t="b">
+        <f>IF(Table2[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H7" t="b">
+        <f>IF(SUM($F$2:$F7)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B8">
@@ -2287,12 +3328,20 @@
         <v>65.351629502572806</v>
       </c>
       <c r="F8" s="1">
-        <f>Table2[[#This Row],[Group-wise Cumulative Percentage]]-E7</f>
-        <v>5.4888507718696076</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+        <f>ROUND(Table2[[#This Row],[Group-wise Cumulative Percentage]]-E7,2)</f>
+        <v>5.49</v>
+      </c>
+      <c r="G8" t="b">
+        <f>IF(Table2[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H8" t="b">
+        <f>IF(SUM($F$2:$F8)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B9">
@@ -2308,12 +3357,20 @@
         <v>70.3259005145797</v>
       </c>
       <c r="F9" s="1">
-        <f>Table2[[#This Row],[Group-wise Cumulative Percentage]]-E8</f>
-        <v>4.9742710120068949</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+        <f>ROUND(Table2[[#This Row],[Group-wise Cumulative Percentage]]-E8,2)</f>
+        <v>4.97</v>
+      </c>
+      <c r="G9" t="b">
+        <f>IF(Table2[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H9" t="b">
+        <f>IF(SUM($F$2:$F9)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B10">
@@ -2329,12 +3386,20 @@
         <v>74.785591766723797</v>
       </c>
       <c r="F10" s="1">
-        <f>Table2[[#This Row],[Group-wise Cumulative Percentage]]-E9</f>
-        <v>4.459691252144097</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+        <f>ROUND(Table2[[#This Row],[Group-wise Cumulative Percentage]]-E9,2)</f>
+        <v>4.46</v>
+      </c>
+      <c r="G10" t="b">
+        <f>IF(Table2[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H10" t="b">
+        <f>IF(SUM($F$2:$F10)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B11">
@@ -2350,11 +3415,19 @@
         <v>79.073756432246995</v>
       </c>
       <c r="F11" s="1">
-        <f>Table2[[#This Row],[Group-wise Cumulative Percentage]]-E10</f>
-        <v>4.2881646655231975</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <f>ROUND(Table2[[#This Row],[Group-wise Cumulative Percentage]]-E10,2)</f>
+        <v>4.29</v>
+      </c>
+      <c r="G11" t="b">
+        <f>IF(Table2[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H11" t="b">
+        <f>IF(SUM($F$2:$F11)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -2371,11 +3444,19 @@
         <v>83.018867924528294</v>
       </c>
       <c r="F12" s="1">
-        <f>Table2[[#This Row],[Group-wise Cumulative Percentage]]-E11</f>
-        <v>3.9451114922812991</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <f>ROUND(Table2[[#This Row],[Group-wise Cumulative Percentage]]-E11,2)</f>
+        <v>3.95</v>
+      </c>
+      <c r="G12" t="b">
+        <f>IF(Table2[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" t="b">
+        <f>IF(SUM($F$2:$F12)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -2392,11 +3473,19 @@
         <v>86.963979416809593</v>
       </c>
       <c r="F13" s="1">
-        <f>Table2[[#This Row],[Group-wise Cumulative Percentage]]-E12</f>
-        <v>3.9451114922812991</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <f>ROUND(Table2[[#This Row],[Group-wise Cumulative Percentage]]-E12,2)</f>
+        <v>3.95</v>
+      </c>
+      <c r="G13" t="b">
+        <f>IF(Table2[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" t="b">
+        <f>IF(SUM($F$2:$F13)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2413,11 +3502,19 @@
         <v>90.394511149228094</v>
       </c>
       <c r="F14" s="1">
-        <f>Table2[[#This Row],[Group-wise Cumulative Percentage]]-E13</f>
-        <v>3.4305317324185012</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <f>ROUND(Table2[[#This Row],[Group-wise Cumulative Percentage]]-E13,2)</f>
+        <v>3.43</v>
+      </c>
+      <c r="G14" t="b">
+        <f>IF(Table2[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <f>IF(SUM($F$2:$F14)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -2434,11 +3531,19 @@
         <v>92.967409948541999</v>
       </c>
       <c r="F15" s="1">
-        <f>Table2[[#This Row],[Group-wise Cumulative Percentage]]-E14</f>
-        <v>2.5728987993139043</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <f>ROUND(Table2[[#This Row],[Group-wise Cumulative Percentage]]-E14,2)</f>
+        <v>2.57</v>
+      </c>
+      <c r="G15" t="b">
+        <f>IF(Table2[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" t="b">
+        <f>IF(SUM($F$2:$F15)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -2455,11 +3560,19 @@
         <v>95.025728987993105</v>
       </c>
       <c r="F16" s="1">
-        <f>Table2[[#This Row],[Group-wise Cumulative Percentage]]-E15</f>
-        <v>2.0583190394511064</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <f>ROUND(Table2[[#This Row],[Group-wise Cumulative Percentage]]-E15,2)</f>
+        <v>2.06</v>
+      </c>
+      <c r="G16" t="b">
+        <f>IF(Table2[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" t="b">
+        <f>IF(SUM($F$2:$F16)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -2476,11 +3589,19 @@
         <v>96.2264150943396</v>
       </c>
       <c r="F17" s="1">
-        <f>Table2[[#This Row],[Group-wise Cumulative Percentage]]-E16</f>
-        <v>1.2006861063464953</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <f>ROUND(Table2[[#This Row],[Group-wise Cumulative Percentage]]-E16,2)</f>
+        <v>1.2</v>
+      </c>
+      <c r="G17" t="b">
+        <f>IF(Table2[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H17" t="b">
+        <f>IF(SUM($F$2:$F17)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -2497,11 +3618,19 @@
         <v>97.427101200686096</v>
       </c>
       <c r="F18" s="1">
-        <f>Table2[[#This Row],[Group-wise Cumulative Percentage]]-E17</f>
-        <v>1.2006861063464953</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <f>ROUND(Table2[[#This Row],[Group-wise Cumulative Percentage]]-E17,2)</f>
+        <v>1.2</v>
+      </c>
+      <c r="G18" t="b">
+        <f>IF(Table2[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" t="b">
+        <f>IF(SUM($F$2:$F18)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -2518,11 +3647,19 @@
         <v>98.456260720411606</v>
       </c>
       <c r="F19" s="1">
-        <f>Table2[[#This Row],[Group-wise Cumulative Percentage]]-E18</f>
-        <v>1.0291595197255106</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <f>ROUND(Table2[[#This Row],[Group-wise Cumulative Percentage]]-E18,2)</f>
+        <v>1.03</v>
+      </c>
+      <c r="G19" t="b">
+        <f>IF(Table2[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
+        <f>IF(SUM($F$2:$F19)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2539,11 +3676,19 @@
         <v>99.313893653516203</v>
       </c>
       <c r="F20" s="1">
-        <f>Table2[[#This Row],[Group-wise Cumulative Percentage]]-E19</f>
-        <v>0.85763293310459687</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <f>ROUND(Table2[[#This Row],[Group-wise Cumulative Percentage]]-E19,2)</f>
+        <v>0.86</v>
+      </c>
+      <c r="G20" t="b">
+        <f>IF(Table2[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H20" t="b">
+        <f>IF(SUM($F$2:$F20)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -2560,15 +3705,155 @@
         <v>100</v>
       </c>
       <c r="F21" s="1">
-        <f>Table2[[#This Row],[Group-wise Cumulative Percentage]]-E20</f>
-        <v>0.68610634648379687</v>
+        <f>ROUND(Table2[[#This Row],[Group-wise Cumulative Percentage]]-E20,2)</f>
+        <v>0.69</v>
+      </c>
+      <c r="G21" t="b">
+        <f>IF(Table2[[#This Row],[Individual]]&gt;=$K$1,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" t="b">
+        <f>IF(SUM($F$2:$F21)&lt;=$K$2,TRUE,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G2:G21">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H21">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F2:F21" calculatedColumn="1"/>
+  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D376B8B-100B-4B12-BB5F-E335748DA596}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="21.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A11">
+    <sortCondition ref="A2:A11"/>
+  </sortState>
+  <conditionalFormatting sqref="B11:C11 C2:C10">
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>